<commit_message>
perbaikan risalah dan tambah field trf_ppn trf_pph trf_ppnbm trf_ppnbm_t trf_bmad trf_bmad_t
</commit_message>
<xml_diff>
--- a/web/uploads/pwdgxDdCWYias4SgMvOBmiEDseAY2swf.xlsx
+++ b/web/uploads/pwdgxDdCWYias4SgMvOBmiEDseAY2swf.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
   <si>
     <t>NpwpImp9</t>
   </si>
@@ -118,6 +118,36 @@
   </si>
   <si>
     <t>Trf pph_t</t>
+  </si>
+  <si>
+    <t>trf_ppn</t>
+  </si>
+  <si>
+    <t>trf_pph</t>
+  </si>
+  <si>
+    <t>trf_ppnbm</t>
+  </si>
+  <si>
+    <t>trf_ppnbm_t</t>
+  </si>
+  <si>
+    <t>trf_bmad</t>
+  </si>
+  <si>
+    <t>trf_bmad_t</t>
+  </si>
+  <si>
+    <t>trf_bk</t>
+  </si>
+  <si>
+    <t>trf_bk_t</t>
+  </si>
+  <si>
+    <t>bk_nilai_awal</t>
+  </si>
+  <si>
+    <t>bk_nilai_akhir</t>
   </si>
 </sst>
 </file>
@@ -486,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA10"/>
+  <dimension ref="A1:AK10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Y8" sqref="Y8"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AJ7" sqref="AJ7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,9 +532,16 @@
     <col min="13" max="13" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="22.140625" customWidth="1"/>
+    <col min="30" max="30" width="10.140625" customWidth="1"/>
+    <col min="31" max="31" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11" customWidth="1"/>
+    <col min="34" max="34" width="11.42578125" customWidth="1"/>
+    <col min="35" max="35" width="9.5703125" customWidth="1"/>
+    <col min="36" max="36" width="15.140625" customWidth="1"/>
+    <col min="37" max="37" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -586,8 +623,38 @@
       <c r="AA1" t="s">
         <v>32</v>
       </c>
+      <c r="AB1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -669,8 +736,38 @@
       <c r="AA2">
         <v>2.5</v>
       </c>
+      <c r="AB2">
+        <v>10</v>
+      </c>
+      <c r="AC2">
+        <v>2.5</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
+        <v>0</v>
+      </c>
+      <c r="AI2">
+        <v>0</v>
+      </c>
+      <c r="AJ2">
+        <v>0</v>
+      </c>
+      <c r="AK2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -752,50 +849,80 @@
       <c r="AA3">
         <v>2.5</v>
       </c>
+      <c r="AB3">
+        <v>10</v>
+      </c>
+      <c r="AC3">
+        <v>2.5</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <v>0</v>
+      </c>
+      <c r="AG3">
+        <v>0</v>
+      </c>
+      <c r="AH3">
+        <v>0</v>
+      </c>
+      <c r="AI3">
+        <v>0</v>
+      </c>
+      <c r="AJ3">
+        <v>0</v>
+      </c>
+      <c r="AK3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="3"/>
       <c r="M4" s="4"/>
       <c r="N4" s="5"/>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="3"/>
       <c r="M5" s="4"/>
       <c r="N5" s="5"/>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="3"/>
       <c r="M6" s="4"/>
       <c r="N6" s="5"/>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="3"/>
       <c r="M7" s="4"/>
       <c r="N7" s="5"/>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="3"/>
       <c r="M8" s="4"/>
       <c r="N8" s="5"/>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="3"/>
       <c r="M9" s="4"/>
       <c r="N9" s="5"/>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="3"/>

</xml_diff>